<commit_message>
feat : api services implemented
</commit_message>
<xml_diff>
--- a/src/Data.Import.Api/ExcelData/Recipe.xlsx
+++ b/src/Data.Import.Api/ExcelData/Recipe.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal Projects\food-recipe-generator-backend\Data.Import.Api\ExcelData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal Projects\food-recipe-generator-backend\src\Data.Import.Api\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE50621A-3B80-43CE-8B63-C77B6C3E4C73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8DBB82B-B1EB-4979-A6A1-4F8B657AFE57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="78">
   <si>
     <t>Ingredient(s)</t>
   </si>
@@ -230,6 +230,30 @@
   </si>
   <si>
     <t>December - January (during harvest festivals)</t>
+  </si>
+  <si>
+    <t>Proteins</t>
+  </si>
+  <si>
+    <t>Fat</t>
+  </si>
+  <si>
+    <t>Carbohydrates</t>
+  </si>
+  <si>
+    <t>Meal Type</t>
+  </si>
+  <si>
+    <t>Preraration Time</t>
+  </si>
+  <si>
+    <t>Cooking Time</t>
+  </si>
+  <si>
+    <t>Image Url</t>
+  </si>
+  <si>
+    <t>https://www.recipetineats.com/wp-content/uploads/2023/10/African-coconut-chicken-curry_3.jpg</t>
   </si>
 </sst>
 </file>
@@ -505,10 +529,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:K40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -516,9 +540,11 @@
     <col min="1" max="1" width="218.88671875" customWidth="1"/>
     <col min="2" max="2" width="41.109375" customWidth="1"/>
     <col min="3" max="3" width="22.44140625" customWidth="1"/>
+    <col min="4" max="4" width="63.33203125" customWidth="1"/>
+    <col min="9" max="9" width="15.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -531,8 +557,29 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -545,8 +592,11 @@
       <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="K2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -560,7 +610,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -574,7 +624,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -588,7 +638,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -602,7 +652,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
@@ -616,7 +666,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
@@ -630,7 +680,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
@@ -644,7 +694,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
@@ -658,7 +708,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
@@ -672,7 +722,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>25</v>
       </c>
@@ -686,7 +736,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>27</v>
       </c>
@@ -700,7 +750,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>29</v>
       </c>
@@ -714,7 +764,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>31</v>
       </c>
@@ -728,7 +778,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>33</v>
       </c>

</xml_diff>